<commit_message>
Added Output Excel for Transaction Status and Update SetTransactionStatus.xaml
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\OneDrive\Documents\UiPath Advance\REF_TabularData\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BF265F-397F-4C2C-BEA8-07440C77F312}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61ED7F8-BFE3-4F02-9068-706B04F9660B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>ManualTransactionThreshold</t>
+  </si>
+  <si>
+    <t>StatusFilePath</t>
+  </si>
+  <si>
+    <t>Data\Output\Status.xlsx</t>
   </si>
 </sst>
 </file>
@@ -538,7 +544,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -615,7 +621,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>